<commit_message>
changed for type 1 pcnt loss deductible
</commit_message>
<xml_diff>
--- a/ftest/data/fm41/Worked_example_policy_calculation_41.xlsx
+++ b/ftest/data/fm41/Worked_example_policy_calculation_41.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\data\fm41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C88E70F-9AB5-48AC-904B-768EAE3EEC50}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECDCDC2-BBC6-4047-9094-1F614E45867F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="480" windowWidth="17280" windowHeight="8916" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,13 @@
     <sheet name="Policy Calculation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="294">
   <si>
     <t>Purpose</t>
   </si>
@@ -1142,9 +1149,6 @@
     <t>Step 1: Net of Location deductible</t>
   </si>
   <si>
-    <t>Location (Amount and % TIV)</t>
-  </si>
-  <si>
     <t>Step 2: Effective Location deductible</t>
   </si>
   <si>
@@ -1161,6 +1165,15 @@
   </si>
   <si>
     <t>Commerical</t>
+  </si>
+  <si>
+    <t>Location (Type 0 = Amout, Type 1 = % Loss, Type 2 = % TIV)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Deductible/limit level</t>
   </si>
 </sst>
 </file>
@@ -1863,12 +1876,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1887,23 +1894,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9809,10 +9822,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IR62"/>
+  <dimension ref="A1:IR63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9860,8 +9873,8 @@
       <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="113" t="s">
-        <v>290</v>
+      <c r="A3" s="108" t="s">
+        <v>289</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -9923,8 +9936,8 @@
       <c r="A7" s="65" t="s">
         <v>233</v>
       </c>
-      <c r="B7" s="103" t="s">
-        <v>291</v>
+      <c r="B7" s="101" t="s">
+        <v>290</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
@@ -10258,22 +10271,22 @@
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="70"/>
       <c r="B28" s="71"/>
-      <c r="C28" s="102" t="s">
+      <c r="C28" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="D28" s="102" t="s">
+      <c r="D28" s="100" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="102" t="s">
+      <c r="E28" s="100" t="s">
         <v>274</v>
       </c>
-      <c r="F28" s="102" t="s">
+      <c r="F28" s="100" t="s">
         <v>275</v>
       </c>
-      <c r="G28" s="102" t="s">
+      <c r="G28" s="100" t="s">
         <v>276</v>
       </c>
-      <c r="H28" s="102" t="s">
+      <c r="H28" s="100" t="s">
         <v>277</v>
       </c>
       <c r="I28" s="71"/>
@@ -10360,28 +10373,28 @@
       <c r="L31" s="62"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="B32" s="103" t="s">
-        <v>285</v>
+      <c r="A32" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>291</v>
       </c>
       <c r="C32" s="61"/>
       <c r="D32" s="61"/>
       <c r="E32" s="61"/>
       <c r="F32" s="61"/>
       <c r="G32" s="61"/>
-      <c r="H32" s="104"/>
+      <c r="H32" s="102"/>
       <c r="I32" s="61"/>
       <c r="J32" s="77"/>
       <c r="K32" s="73"/>
       <c r="L32" s="62"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="105" t="s">
+      <c r="A33" s="103" t="s">
         <v>259</v>
       </c>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="101" t="s">
         <v>278</v>
       </c>
       <c r="C33" s="61">
@@ -10399,7 +10412,7 @@
       <c r="G33" s="61">
         <v>10000</v>
       </c>
-      <c r="H33" s="104">
+      <c r="H33" s="102">
         <v>0.1</v>
       </c>
       <c r="I33" s="61"/>
@@ -10408,54 +10421,62 @@
       <c r="L33" s="62"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="B34" s="103" t="s">
-        <v>279</v>
-      </c>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
+      <c r="A34" s="103" t="s">
+        <v>292</v>
+      </c>
+      <c r="B34" s="101"/>
+      <c r="C34" s="61">
+        <v>0</v>
+      </c>
+      <c r="D34" s="61">
+        <v>2</v>
+      </c>
+      <c r="E34" s="61">
+        <v>1</v>
+      </c>
+      <c r="F34" s="61">
+        <v>0</v>
+      </c>
+      <c r="G34" s="61">
+        <v>0</v>
+      </c>
+      <c r="H34" s="102">
+        <v>2</v>
+      </c>
       <c r="I34" s="61"/>
       <c r="J34" s="82"/>
       <c r="K34" s="73"/>
       <c r="L34" s="62"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="106" t="s">
-        <v>280</v>
-      </c>
-      <c r="B35" s="61"/>
-      <c r="C35" s="110">
-        <v>1</v>
-      </c>
-      <c r="D35" s="108"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
+      <c r="A35" s="103" t="s">
+        <v>293</v>
+      </c>
+      <c r="B35" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" s="110"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="110"/>
       <c r="I35" s="61"/>
-      <c r="J35" s="77"/>
+      <c r="J35" s="82"/>
       <c r="K35" s="73"/>
       <c r="L35" s="62"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="106" t="s">
-        <v>281</v>
-      </c>
-      <c r="B36" s="112" t="s">
-        <v>282</v>
-      </c>
-      <c r="C36" s="110">
-        <v>50000</v>
-      </c>
-      <c r="D36" s="108"/>
-      <c r="E36" s="111"/>
-      <c r="F36" s="109"/>
+      <c r="A36" s="104" t="s">
+        <v>280</v>
+      </c>
+      <c r="B36" s="61"/>
+      <c r="C36" s="111">
+        <v>1</v>
+      </c>
+      <c r="D36" s="112"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="106"/>
       <c r="G36" s="83"/>
       <c r="H36" s="83"/>
       <c r="I36" s="61"/>
@@ -10464,18 +10485,18 @@
       <c r="L36" s="62"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="106" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" s="112" t="s">
-        <v>261</v>
-      </c>
-      <c r="C37" s="110">
-        <v>250000</v>
-      </c>
-      <c r="D37" s="108"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="109"/>
+      <c r="A37" s="104" t="s">
+        <v>281</v>
+      </c>
+      <c r="B37" s="107" t="s">
+        <v>282</v>
+      </c>
+      <c r="C37" s="111">
+        <v>50000</v>
+      </c>
+      <c r="D37" s="112"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="106"/>
       <c r="G37" s="83"/>
       <c r="H37" s="83"/>
       <c r="I37" s="61"/>
@@ -10484,16 +10505,18 @@
       <c r="L37" s="62"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="B38" s="112" t="s">
-        <v>251</v>
-      </c>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="83"/>
+      <c r="A38" s="104" t="s">
+        <v>260</v>
+      </c>
+      <c r="B38" s="107" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="111">
+        <v>250000</v>
+      </c>
+      <c r="D38" s="112"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="106"/>
       <c r="G38" s="83"/>
       <c r="H38" s="83"/>
       <c r="I38" s="61"/>
@@ -10502,380 +10525,364 @@
       <c r="L38" s="62"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="106" t="s">
-        <v>260</v>
-      </c>
-      <c r="B39" s="112" t="s">
-        <v>283</v>
-      </c>
-      <c r="C39" s="107"/>
-      <c r="D39" s="107"/>
-      <c r="E39" s="107"/>
+      <c r="A39" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="B39" s="107" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
       <c r="F39" s="83"/>
       <c r="G39" s="83"/>
       <c r="H39" s="83"/>
       <c r="I39" s="61"/>
-      <c r="J39" s="82">
-        <v>1500000</v>
-      </c>
+      <c r="J39" s="77"/>
       <c r="K39" s="73"/>
       <c r="L39" s="62"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="74" t="s">
-        <v>262</v>
-      </c>
-      <c r="B40" s="69"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="84"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="84"/>
+      <c r="A40" s="104" t="s">
+        <v>260</v>
+      </c>
+      <c r="B40" s="107" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" s="105"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
       <c r="I40" s="61"/>
-      <c r="J40" s="77"/>
+      <c r="J40" s="82">
+        <v>1500000</v>
+      </c>
       <c r="K40" s="73"/>
       <c r="L40" s="62"/>
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="78" t="s">
-        <v>263</v>
-      </c>
-      <c r="B41" s="85" t="s">
-        <v>264</v>
-      </c>
-      <c r="C41" s="86">
-        <v>1</v>
-      </c>
-      <c r="D41" s="86">
-        <v>1</v>
-      </c>
-      <c r="E41" s="86">
-        <v>1</v>
-      </c>
-      <c r="F41" s="86">
-        <v>1</v>
-      </c>
-      <c r="G41" s="86">
-        <v>1</v>
-      </c>
-      <c r="H41" s="86">
-        <v>1</v>
-      </c>
+      <c r="A41" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" s="69"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
       <c r="I41" s="61"/>
       <c r="J41" s="77"/>
       <c r="K41" s="73"/>
       <c r="L41" s="62"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="73"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="83"/>
-      <c r="D42" s="83"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="83"/>
-      <c r="H42" s="83"/>
+      <c r="A42" s="78" t="s">
+        <v>263</v>
+      </c>
+      <c r="B42" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="C42" s="86">
+        <v>1</v>
+      </c>
+      <c r="D42" s="86">
+        <v>1</v>
+      </c>
+      <c r="E42" s="86">
+        <v>1</v>
+      </c>
+      <c r="F42" s="86">
+        <v>1</v>
+      </c>
+      <c r="G42" s="86">
+        <v>1</v>
+      </c>
+      <c r="H42" s="86">
+        <v>1</v>
+      </c>
       <c r="I42" s="61"/>
       <c r="J42" s="77"/>
       <c r="K42" s="73"/>
       <c r="L42" s="62"/>
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="74" t="s">
-        <v>265</v>
-      </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="84"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
       <c r="I43" s="61"/>
-      <c r="J43" s="87" t="s">
-        <v>266</v>
-      </c>
+      <c r="J43" s="77"/>
       <c r="K43" s="73"/>
       <c r="L43" s="62"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="78" t="s">
-        <v>267</v>
-      </c>
-      <c r="B44" s="85" t="s">
-        <v>268</v>
-      </c>
-      <c r="C44" s="88">
-        <f>C41*C31</f>
-        <v>1000000</v>
-      </c>
-      <c r="D44" s="88">
-        <f>D41*D31</f>
-        <v>1000000</v>
-      </c>
-      <c r="E44" s="88">
-        <f>E41*E31</f>
-        <v>1000000</v>
-      </c>
-      <c r="F44" s="88">
-        <f>F41*F31</f>
-        <v>2000000</v>
-      </c>
-      <c r="G44" s="88">
-        <f>G41*G31</f>
-        <v>2000000</v>
-      </c>
-      <c r="H44" s="88">
-        <f>H41*H31</f>
-        <v>2000000</v>
-      </c>
+      <c r="A44" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" s="69"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="84"/>
       <c r="I44" s="61"/>
-      <c r="J44" s="89">
-        <f>SUM(C44:H44)</f>
-        <v>9000000</v>
+      <c r="J44" s="87" t="s">
+        <v>266</v>
       </c>
       <c r="K44" s="73"/>
       <c r="L44" s="62"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="105" t="s">
-        <v>284</v>
-      </c>
-      <c r="B45" s="66" t="s">
-        <v>269</v>
-      </c>
-      <c r="C45" s="94">
-        <f>MAX(C44-IF(C33&lt;1,C33*C31,C33),0)</f>
-        <v>990000</v>
-      </c>
-      <c r="D45" s="94">
-        <f>MAX(D44-IF(D33&lt;1,D33*D31,D33),0)</f>
-        <v>990000</v>
-      </c>
-      <c r="E45" s="94">
-        <f t="shared" ref="E45:H45" si="0">MAX(E44-IF(E33&lt;1,E33*E31,E33),0)</f>
-        <v>950000</v>
-      </c>
-      <c r="F45" s="94">
-        <f>MAX(F44-IF(F33&lt;1,F33*F31,F33),0)</f>
-        <v>1985000</v>
-      </c>
-      <c r="G45" s="94">
-        <f>MAX(G44-IF(G33&lt;1,G33*G31,G33),0)</f>
-        <v>1990000</v>
-      </c>
-      <c r="H45" s="94">
+      <c r="A45" s="78" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="85" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="88">
+        <f t="shared" ref="C45:H45" si="0">C42*C31</f>
+        <v>1000000</v>
+      </c>
+      <c r="D45" s="88">
         <f t="shared" si="0"/>
-        <v>1800000</v>
+        <v>1000000</v>
+      </c>
+      <c r="E45" s="88">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="F45" s="88">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="G45" s="88">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="H45" s="88">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
       </c>
       <c r="I45" s="61"/>
-      <c r="J45" s="91">
+      <c r="J45" s="89">
         <f>SUM(C45:H45)</f>
-        <v>8705000</v>
+        <v>9000000</v>
       </c>
       <c r="K45" s="73"/>
       <c r="L45" s="62"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="105" t="s">
-        <v>286</v>
-      </c>
-      <c r="B46" s="66"/>
+      <c r="A46" s="103" t="s">
+        <v>284</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>269</v>
+      </c>
       <c r="C46" s="94">
-        <f>C44-C45</f>
-        <v>10000</v>
+        <f>MAX(C45-IF(C34=2,C33*C31,IF(C34=1,C45*C33,C33)),0)</f>
+        <v>990000</v>
       </c>
       <c r="D46" s="94">
-        <f t="shared" ref="D46:H46" si="1">D44-D45</f>
-        <v>10000</v>
+        <f>MAX(D45-IF(D34=2,D33*D31,IF(D34=1,D45*D33,D33)),0)</f>
+        <v>990000</v>
       </c>
       <c r="E46" s="94">
-        <f t="shared" si="1"/>
-        <v>50000</v>
+        <f>MAX(E45-IF(E34=2,E33*E31,IF(E34=1,E45*E33,E33)),0)</f>
+        <v>950000</v>
       </c>
       <c r="F46" s="94">
-        <f t="shared" si="1"/>
-        <v>15000</v>
+        <f>MAX(F45-IF(F34=2,F33*F31,IF(F34=1,F45*F33,F33)),0)</f>
+        <v>1985000</v>
       </c>
       <c r="G46" s="94">
-        <f t="shared" si="1"/>
-        <v>10000</v>
+        <f>MAX(G45-IF(G34=2,G33*G31,IF(G34=1,G45*G33,G33)),0)</f>
+        <v>1990000</v>
       </c>
       <c r="H46" s="94">
-        <f t="shared" si="1"/>
-        <v>200000</v>
+        <f>MAX(H45-IF(H34=2,H33*H31,IF(H34=1,H45*H33,H33)),0)</f>
+        <v>1800000</v>
       </c>
       <c r="I46" s="61"/>
       <c r="J46" s="91">
         <f>SUM(C46:H46)</f>
-        <v>295000</v>
+        <v>8705000</v>
       </c>
       <c r="K46" s="73"/>
       <c r="L46" s="62"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="105" t="s">
-        <v>287</v>
+      <c r="A47" s="103" t="s">
+        <v>285</v>
       </c>
       <c r="B47" s="66"/>
-      <c r="C47" s="100">
-        <f>MIN(MAX(C36,SUM(C46:E46)),SUM(C44:E44))</f>
-        <v>70000</v>
-      </c>
-      <c r="D47" s="100"/>
-      <c r="E47" s="100"/>
-      <c r="F47" s="100">
-        <v>0</v>
-      </c>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
+      <c r="C47" s="94">
+        <f>C45-C46</f>
+        <v>10000</v>
+      </c>
+      <c r="D47" s="94">
+        <f t="shared" ref="D47:H47" si="1">D45-D46</f>
+        <v>10000</v>
+      </c>
+      <c r="E47" s="94">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="F47" s="94">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="G47" s="94">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="H47" s="94">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
       <c r="I47" s="61"/>
-      <c r="J47" s="91"/>
+      <c r="J47" s="91">
+        <f>SUM(C47:H47)</f>
+        <v>295000</v>
+      </c>
       <c r="K47" s="73"/>
       <c r="L47" s="62"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="105" t="s">
-        <v>288</v>
+      <c r="A48" s="103" t="s">
+        <v>286</v>
       </c>
       <c r="B48" s="66"/>
-      <c r="C48" s="100">
-        <f>MIN(C37,MAX(SUM(C44:E44)-C47,0))</f>
-        <v>250000</v>
-      </c>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100">
-        <f>SUM(F45:H45)</f>
-        <v>5775000</v>
-      </c>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
+      <c r="C48" s="109">
+        <f>MIN(MAX(C37,SUM(C47:E47)),SUM(C45:E45))</f>
+        <v>70000</v>
+      </c>
+      <c r="D48" s="109"/>
+      <c r="E48" s="109"/>
+      <c r="F48" s="109">
+        <v>0</v>
+      </c>
+      <c r="G48" s="109"/>
+      <c r="H48" s="109"/>
       <c r="I48" s="61"/>
-      <c r="J48" s="91">
-        <f>SUM(C48:H48)</f>
-        <v>6025000</v>
-      </c>
+      <c r="J48" s="91"/>
       <c r="K48" s="73"/>
       <c r="L48" s="62"/>
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="105" t="s">
-        <v>289</v>
+      <c r="A49" s="103" t="s">
+        <v>287</v>
       </c>
       <c r="B49" s="66"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
+      <c r="C49" s="109">
+        <f>MIN(C38,MAX(SUM(C45:E45)-C48,0))</f>
+        <v>250000</v>
+      </c>
+      <c r="D49" s="109"/>
+      <c r="E49" s="109"/>
+      <c r="F49" s="109">
+        <f>SUM(F46:H46)</f>
+        <v>5775000</v>
+      </c>
+      <c r="G49" s="109"/>
+      <c r="H49" s="109"/>
       <c r="I49" s="61"/>
       <c r="J49" s="91">
-        <f>MIN(J48,J39)</f>
-        <v>1500000</v>
+        <f>SUM(C49:H49)</f>
+        <v>6025000</v>
       </c>
       <c r="K49" s="73"/>
       <c r="L49" s="62"/>
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="74" t="s">
-        <v>270</v>
-      </c>
-      <c r="B50" s="75" t="s">
-        <v>271</v>
-      </c>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="92">
-        <f>J49</f>
+      <c r="A50" s="103" t="s">
+        <v>288</v>
+      </c>
+      <c r="B50" s="66"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="91">
+        <f>MIN(J49,J40)</f>
         <v>1500000</v>
       </c>
       <c r="K50" s="73"/>
       <c r="L50" s="62"/>
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="93"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="61"/>
+      <c r="A51" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="B51" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+      <c r="J51" s="92">
+        <f>J50</f>
+        <v>1500000</v>
+      </c>
+      <c r="K51" s="73"/>
       <c r="L51" s="62"/>
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="B52" s="61"/>
-      <c r="C52" s="94">
-        <f>$J$50*C44/SUM($C$44:$H$44)</f>
-        <v>166666.66666666666</v>
-      </c>
-      <c r="D52" s="94">
-        <f>$J$50*D44/SUM($C$44:$H$44)</f>
-        <v>166666.66666666666</v>
-      </c>
-      <c r="E52" s="81">
-        <f>$J$50*E44/SUM($C$44:$H$44)</f>
-        <v>166666.66666666666</v>
-      </c>
-      <c r="F52" s="81">
-        <f>$J$50*F44/SUM($C$44:$H$44)</f>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="G52" s="81">
-        <f>$J$50*G44/SUM($C$44:$H$44)</f>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="H52" s="81">
-        <f>$J$50*H44/SUM($C$44:$H$44)</f>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="I52" s="61"/>
-      <c r="J52" s="61"/>
+      <c r="A52" s="93"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="71"/>
+      <c r="H52" s="71"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="71"/>
       <c r="K52" s="61"/>
       <c r="L52" s="62"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B53" s="61"/>
       <c r="C53" s="94">
-        <f>IFERROR($J$50*C45/SUM($C$45:$E$45)*$C$48/$J$48,0)</f>
-        <v>21030.121932222111</v>
+        <f t="shared" ref="C53:H53" si="2">$J$51*C45/SUM($C$45:$H$45)</f>
+        <v>166666.66666666666</v>
       </c>
       <c r="D53" s="94">
-        <f t="shared" ref="D53:E53" si="2">IFERROR($J$50*D45/SUM($C$45:$E$45)*$C$48/$J$48,0)</f>
-        <v>21030.121932222111</v>
-      </c>
-      <c r="E53" s="94">
         <f t="shared" si="2"/>
-        <v>20180.420035970714</v>
-      </c>
-      <c r="F53" s="94">
-        <f>IFERROR($J$50*F45/SUM($F$45:$H$45)*$F$48/$J$48,0)</f>
-        <v>494190.87136929459</v>
-      </c>
-      <c r="G53" s="94">
-        <f t="shared" ref="G53:H53" si="3">IFERROR($J$50*G45/SUM($F$45:$H$45)*$F$48/$J$48,0)</f>
-        <v>495435.6846473029</v>
-      </c>
-      <c r="H53" s="94">
-        <f t="shared" si="3"/>
-        <v>448132.78008298756</v>
+        <v>166666.66666666666</v>
+      </c>
+      <c r="E53" s="81">
+        <f t="shared" si="2"/>
+        <v>166666.66666666666</v>
+      </c>
+      <c r="F53" s="81">
+        <f t="shared" si="2"/>
+        <v>333333.33333333331</v>
+      </c>
+      <c r="G53" s="81">
+        <f t="shared" si="2"/>
+        <v>333333.33333333331</v>
+      </c>
+      <c r="H53" s="81">
+        <f t="shared" si="2"/>
+        <v>333333.33333333331</v>
       </c>
       <c r="I53" s="61"/>
       <c r="J53" s="61"/>
@@ -10883,14 +10890,34 @@
       <c r="L53" s="62"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="63"/>
+      <c r="A54" s="11" t="s">
+        <v>273</v>
+      </c>
       <c r="B54" s="61"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="61"/>
+      <c r="C54" s="94">
+        <f>IFERROR($J$51*C46/SUM($C$46:$E$46)*$C$49/$J$49,0)</f>
+        <v>21030.121932222111</v>
+      </c>
+      <c r="D54" s="94">
+        <f t="shared" ref="D54:E54" si="3">IFERROR($J$51*D46/SUM($C$46:$E$46)*$C$49/$J$49,0)</f>
+        <v>21030.121932222111</v>
+      </c>
+      <c r="E54" s="94">
+        <f t="shared" si="3"/>
+        <v>20180.420035970714</v>
+      </c>
+      <c r="F54" s="94">
+        <f>IFERROR($J$51*F46/SUM($F$46:$H$46)*$F$49/$J$49,0)</f>
+        <v>494190.87136929459</v>
+      </c>
+      <c r="G54" s="94">
+        <f t="shared" ref="G54:H54" si="4">IFERROR($J$51*G46/SUM($F$46:$H$46)*$F$49/$J$49,0)</f>
+        <v>495435.6846473029</v>
+      </c>
+      <c r="H54" s="94">
+        <f t="shared" si="4"/>
+        <v>448132.78008298756</v>
+      </c>
       <c r="I54" s="61"/>
       <c r="J54" s="61"/>
       <c r="K54" s="61"/>
@@ -10899,7 +10926,7 @@
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="63"/>
       <c r="B55" s="61"/>
-      <c r="C55" s="95"/>
+      <c r="C55" s="61"/>
       <c r="D55" s="61"/>
       <c r="E55" s="61"/>
       <c r="F55" s="61"/>
@@ -10995,30 +11022,44 @@
       <c r="L61" s="62"/>
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="96"/>
-      <c r="B62" s="97"/>
-      <c r="C62" s="98"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="97"/>
-      <c r="F62" s="97"/>
-      <c r="G62" s="97"/>
-      <c r="H62" s="97"/>
-      <c r="I62" s="97"/>
-      <c r="J62" s="97"/>
-      <c r="K62" s="97"/>
-      <c r="L62" s="99"/>
+      <c r="A62" s="63"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="62"/>
+    </row>
+    <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="96"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="97"/>
+      <c r="G63" s="97"/>
+      <c r="H63" s="97"/>
+      <c r="I63" s="97"/>
+      <c r="J63" s="97"/>
+      <c r="K63" s="97"/>
+      <c r="L63" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
     <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C35:E35"/>
   </mergeCells>
   <pageMargins left="0.70866099999999999" right="0.70866099999999999" top="0.748031" bottom="0.748031" header="0.31496099999999999" footer="0.31496099999999999"/>
   <pageSetup scale="44" orientation="portrait"/>

</xml_diff>

<commit_message>
updated for type 1
</commit_message>
<xml_diff>
--- a/ftest/data/fm41/Worked_example_policy_calculation_41.xlsx
+++ b/ftest/data/fm41/Worked_example_policy_calculation_41.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest\ftest\data\fm41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECDCDC2-BBC6-4047-9094-1F614E45867F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517DE66-C8DD-4A59-9F34-13F14CEEF4CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1294,12 +1294,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="23"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="24"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1307,6 +1301,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1661,7 +1661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1838,7 +1838,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="16" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1879,44 +1879,73 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="18" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9824,8 +9853,8 @@
   </sheetPr>
   <dimension ref="A1:IR63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9873,7 +9902,7 @@
       <c r="L2" s="62"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="107" t="s">
         <v>289</v>
       </c>
       <c r="B3" s="61"/>
@@ -10390,145 +10419,1585 @@
       <c r="K32" s="73"/>
       <c r="L32" s="62"/>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="103" t="s">
+    <row r="33" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="109" t="s">
         <v>259</v>
       </c>
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="110" t="s">
         <v>278</v>
       </c>
-      <c r="C33" s="61">
+      <c r="C33" s="111">
         <v>10000</v>
       </c>
-      <c r="D33" s="61">
+      <c r="D33" s="111">
         <v>0.01</v>
       </c>
-      <c r="E33" s="61">
+      <c r="E33" s="111">
         <v>0.05</v>
       </c>
-      <c r="F33" s="61">
+      <c r="F33" s="111">
         <v>15000</v>
       </c>
-      <c r="G33" s="61">
+      <c r="G33" s="111">
         <v>10000</v>
       </c>
-      <c r="H33" s="102">
+      <c r="H33" s="112">
         <v>0.1</v>
       </c>
-      <c r="I33" s="61"/>
-      <c r="J33" s="82"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="62"/>
-    </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="103" t="s">
+      <c r="I33" s="111"/>
+      <c r="J33" s="113"/>
+      <c r="K33" s="114"/>
+      <c r="L33" s="115"/>
+      <c r="M33" s="116"/>
+      <c r="N33" s="116"/>
+      <c r="O33" s="116"/>
+      <c r="P33" s="116"/>
+      <c r="Q33" s="116"/>
+      <c r="R33" s="116"/>
+      <c r="S33" s="116"/>
+      <c r="T33" s="116"/>
+      <c r="U33" s="116"/>
+      <c r="V33" s="116"/>
+      <c r="W33" s="116"/>
+      <c r="X33" s="116"/>
+      <c r="Y33" s="116"/>
+      <c r="Z33" s="116"/>
+      <c r="AA33" s="116"/>
+      <c r="AB33" s="116"/>
+      <c r="AC33" s="116"/>
+      <c r="AD33" s="116"/>
+      <c r="AE33" s="116"/>
+      <c r="AF33" s="116"/>
+      <c r="AG33" s="116"/>
+      <c r="AH33" s="116"/>
+      <c r="AI33" s="116"/>
+      <c r="AJ33" s="116"/>
+      <c r="AK33" s="116"/>
+      <c r="AL33" s="116"/>
+      <c r="AM33" s="116"/>
+      <c r="AN33" s="116"/>
+      <c r="AO33" s="116"/>
+      <c r="AP33" s="116"/>
+      <c r="AQ33" s="116"/>
+      <c r="AR33" s="116"/>
+      <c r="AS33" s="116"/>
+      <c r="AT33" s="116"/>
+      <c r="AU33" s="116"/>
+      <c r="AV33" s="116"/>
+      <c r="AW33" s="116"/>
+      <c r="AX33" s="116"/>
+      <c r="AY33" s="116"/>
+      <c r="AZ33" s="116"/>
+      <c r="BA33" s="116"/>
+      <c r="BB33" s="116"/>
+      <c r="BC33" s="116"/>
+      <c r="BD33" s="116"/>
+      <c r="BE33" s="116"/>
+      <c r="BF33" s="116"/>
+      <c r="BG33" s="116"/>
+      <c r="BH33" s="116"/>
+      <c r="BI33" s="116"/>
+      <c r="BJ33" s="116"/>
+      <c r="BK33" s="116"/>
+      <c r="BL33" s="116"/>
+      <c r="BM33" s="116"/>
+      <c r="BN33" s="116"/>
+      <c r="BO33" s="116"/>
+      <c r="BP33" s="116"/>
+      <c r="BQ33" s="116"/>
+      <c r="BR33" s="116"/>
+      <c r="BS33" s="116"/>
+      <c r="BT33" s="116"/>
+      <c r="BU33" s="116"/>
+      <c r="BV33" s="116"/>
+      <c r="BW33" s="116"/>
+      <c r="BX33" s="116"/>
+      <c r="BY33" s="116"/>
+      <c r="BZ33" s="116"/>
+      <c r="CA33" s="116"/>
+      <c r="CB33" s="116"/>
+      <c r="CC33" s="116"/>
+      <c r="CD33" s="116"/>
+      <c r="CE33" s="116"/>
+      <c r="CF33" s="116"/>
+      <c r="CG33" s="116"/>
+      <c r="CH33" s="116"/>
+      <c r="CI33" s="116"/>
+      <c r="CJ33" s="116"/>
+      <c r="CK33" s="116"/>
+      <c r="CL33" s="116"/>
+      <c r="CM33" s="116"/>
+      <c r="CN33" s="116"/>
+      <c r="CO33" s="116"/>
+      <c r="CP33" s="116"/>
+      <c r="CQ33" s="116"/>
+      <c r="CR33" s="116"/>
+      <c r="CS33" s="116"/>
+      <c r="CT33" s="116"/>
+      <c r="CU33" s="116"/>
+      <c r="CV33" s="116"/>
+      <c r="CW33" s="116"/>
+      <c r="CX33" s="116"/>
+      <c r="CY33" s="116"/>
+      <c r="CZ33" s="116"/>
+      <c r="DA33" s="116"/>
+      <c r="DB33" s="116"/>
+      <c r="DC33" s="116"/>
+      <c r="DD33" s="116"/>
+      <c r="DE33" s="116"/>
+      <c r="DF33" s="116"/>
+      <c r="DG33" s="116"/>
+      <c r="DH33" s="116"/>
+      <c r="DI33" s="116"/>
+      <c r="DJ33" s="116"/>
+      <c r="DK33" s="116"/>
+      <c r="DL33" s="116"/>
+      <c r="DM33" s="116"/>
+      <c r="DN33" s="116"/>
+      <c r="DO33" s="116"/>
+      <c r="DP33" s="116"/>
+      <c r="DQ33" s="116"/>
+      <c r="DR33" s="116"/>
+      <c r="DS33" s="116"/>
+      <c r="DT33" s="116"/>
+      <c r="DU33" s="116"/>
+      <c r="DV33" s="116"/>
+      <c r="DW33" s="116"/>
+      <c r="DX33" s="116"/>
+      <c r="DY33" s="116"/>
+      <c r="DZ33" s="116"/>
+      <c r="EA33" s="116"/>
+      <c r="EB33" s="116"/>
+      <c r="EC33" s="116"/>
+      <c r="ED33" s="116"/>
+      <c r="EE33" s="116"/>
+      <c r="EF33" s="116"/>
+      <c r="EG33" s="116"/>
+      <c r="EH33" s="116"/>
+      <c r="EI33" s="116"/>
+      <c r="EJ33" s="116"/>
+      <c r="EK33" s="116"/>
+      <c r="EL33" s="116"/>
+      <c r="EM33" s="116"/>
+      <c r="EN33" s="116"/>
+      <c r="EO33" s="116"/>
+      <c r="EP33" s="116"/>
+      <c r="EQ33" s="116"/>
+      <c r="ER33" s="116"/>
+      <c r="ES33" s="116"/>
+      <c r="ET33" s="116"/>
+      <c r="EU33" s="116"/>
+      <c r="EV33" s="116"/>
+      <c r="EW33" s="116"/>
+      <c r="EX33" s="116"/>
+      <c r="EY33" s="116"/>
+      <c r="EZ33" s="116"/>
+      <c r="FA33" s="116"/>
+      <c r="FB33" s="116"/>
+      <c r="FC33" s="116"/>
+      <c r="FD33" s="116"/>
+      <c r="FE33" s="116"/>
+      <c r="FF33" s="116"/>
+      <c r="FG33" s="116"/>
+      <c r="FH33" s="116"/>
+      <c r="FI33" s="116"/>
+      <c r="FJ33" s="116"/>
+      <c r="FK33" s="116"/>
+      <c r="FL33" s="116"/>
+      <c r="FM33" s="116"/>
+      <c r="FN33" s="116"/>
+      <c r="FO33" s="116"/>
+      <c r="FP33" s="116"/>
+      <c r="FQ33" s="116"/>
+      <c r="FR33" s="116"/>
+      <c r="FS33" s="116"/>
+      <c r="FT33" s="116"/>
+      <c r="FU33" s="116"/>
+      <c r="FV33" s="116"/>
+      <c r="FW33" s="116"/>
+      <c r="FX33" s="116"/>
+      <c r="FY33" s="116"/>
+      <c r="FZ33" s="116"/>
+      <c r="GA33" s="116"/>
+      <c r="GB33" s="116"/>
+      <c r="GC33" s="116"/>
+      <c r="GD33" s="116"/>
+      <c r="GE33" s="116"/>
+      <c r="GF33" s="116"/>
+      <c r="GG33" s="116"/>
+      <c r="GH33" s="116"/>
+      <c r="GI33" s="116"/>
+      <c r="GJ33" s="116"/>
+      <c r="GK33" s="116"/>
+      <c r="GL33" s="116"/>
+      <c r="GM33" s="116"/>
+      <c r="GN33" s="116"/>
+      <c r="GO33" s="116"/>
+      <c r="GP33" s="116"/>
+      <c r="GQ33" s="116"/>
+      <c r="GR33" s="116"/>
+      <c r="GS33" s="116"/>
+      <c r="GT33" s="116"/>
+      <c r="GU33" s="116"/>
+      <c r="GV33" s="116"/>
+      <c r="GW33" s="116"/>
+      <c r="GX33" s="116"/>
+      <c r="GY33" s="116"/>
+      <c r="GZ33" s="116"/>
+      <c r="HA33" s="116"/>
+      <c r="HB33" s="116"/>
+      <c r="HC33" s="116"/>
+      <c r="HD33" s="116"/>
+      <c r="HE33" s="116"/>
+      <c r="HF33" s="116"/>
+      <c r="HG33" s="116"/>
+      <c r="HH33" s="116"/>
+      <c r="HI33" s="116"/>
+      <c r="HJ33" s="116"/>
+      <c r="HK33" s="116"/>
+      <c r="HL33" s="116"/>
+      <c r="HM33" s="116"/>
+      <c r="HN33" s="116"/>
+      <c r="HO33" s="116"/>
+      <c r="HP33" s="116"/>
+      <c r="HQ33" s="116"/>
+      <c r="HR33" s="116"/>
+      <c r="HS33" s="116"/>
+      <c r="HT33" s="116"/>
+      <c r="HU33" s="116"/>
+      <c r="HV33" s="116"/>
+      <c r="HW33" s="116"/>
+      <c r="HX33" s="116"/>
+      <c r="HY33" s="116"/>
+      <c r="HZ33" s="116"/>
+      <c r="IA33" s="116"/>
+      <c r="IB33" s="116"/>
+      <c r="IC33" s="116"/>
+      <c r="ID33" s="116"/>
+      <c r="IE33" s="116"/>
+      <c r="IF33" s="116"/>
+      <c r="IG33" s="116"/>
+      <c r="IH33" s="116"/>
+      <c r="II33" s="116"/>
+      <c r="IJ33" s="116"/>
+      <c r="IK33" s="116"/>
+      <c r="IL33" s="116"/>
+      <c r="IM33" s="116"/>
+      <c r="IN33" s="116"/>
+      <c r="IO33" s="116"/>
+      <c r="IP33" s="116"/>
+      <c r="IQ33" s="116"/>
+      <c r="IR33" s="116"/>
+    </row>
+    <row r="34" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="109" t="s">
         <v>292</v>
       </c>
-      <c r="B34" s="101"/>
-      <c r="C34" s="61">
-        <v>0</v>
-      </c>
-      <c r="D34" s="61">
+      <c r="B34" s="110"/>
+      <c r="C34" s="111">
+        <v>0</v>
+      </c>
+      <c r="D34" s="111">
         <v>2</v>
       </c>
-      <c r="E34" s="61">
+      <c r="E34" s="111">
         <v>1</v>
       </c>
-      <c r="F34" s="61">
-        <v>0</v>
-      </c>
-      <c r="G34" s="61">
-        <v>0</v>
-      </c>
-      <c r="H34" s="102">
+      <c r="F34" s="111">
+        <v>0</v>
+      </c>
+      <c r="G34" s="111">
+        <v>0</v>
+      </c>
+      <c r="H34" s="112">
         <v>2</v>
       </c>
-      <c r="I34" s="61"/>
-      <c r="J34" s="82"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="62"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="103" t="s">
+      <c r="I34" s="111"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="114"/>
+      <c r="L34" s="115"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
+      <c r="O34" s="116"/>
+      <c r="P34" s="116"/>
+      <c r="Q34" s="116"/>
+      <c r="R34" s="116"/>
+      <c r="S34" s="116"/>
+      <c r="T34" s="116"/>
+      <c r="U34" s="116"/>
+      <c r="V34" s="116"/>
+      <c r="W34" s="116"/>
+      <c r="X34" s="116"/>
+      <c r="Y34" s="116"/>
+      <c r="Z34" s="116"/>
+      <c r="AA34" s="116"/>
+      <c r="AB34" s="116"/>
+      <c r="AC34" s="116"/>
+      <c r="AD34" s="116"/>
+      <c r="AE34" s="116"/>
+      <c r="AF34" s="116"/>
+      <c r="AG34" s="116"/>
+      <c r="AH34" s="116"/>
+      <c r="AI34" s="116"/>
+      <c r="AJ34" s="116"/>
+      <c r="AK34" s="116"/>
+      <c r="AL34" s="116"/>
+      <c r="AM34" s="116"/>
+      <c r="AN34" s="116"/>
+      <c r="AO34" s="116"/>
+      <c r="AP34" s="116"/>
+      <c r="AQ34" s="116"/>
+      <c r="AR34" s="116"/>
+      <c r="AS34" s="116"/>
+      <c r="AT34" s="116"/>
+      <c r="AU34" s="116"/>
+      <c r="AV34" s="116"/>
+      <c r="AW34" s="116"/>
+      <c r="AX34" s="116"/>
+      <c r="AY34" s="116"/>
+      <c r="AZ34" s="116"/>
+      <c r="BA34" s="116"/>
+      <c r="BB34" s="116"/>
+      <c r="BC34" s="116"/>
+      <c r="BD34" s="116"/>
+      <c r="BE34" s="116"/>
+      <c r="BF34" s="116"/>
+      <c r="BG34" s="116"/>
+      <c r="BH34" s="116"/>
+      <c r="BI34" s="116"/>
+      <c r="BJ34" s="116"/>
+      <c r="BK34" s="116"/>
+      <c r="BL34" s="116"/>
+      <c r="BM34" s="116"/>
+      <c r="BN34" s="116"/>
+      <c r="BO34" s="116"/>
+      <c r="BP34" s="116"/>
+      <c r="BQ34" s="116"/>
+      <c r="BR34" s="116"/>
+      <c r="BS34" s="116"/>
+      <c r="BT34" s="116"/>
+      <c r="BU34" s="116"/>
+      <c r="BV34" s="116"/>
+      <c r="BW34" s="116"/>
+      <c r="BX34" s="116"/>
+      <c r="BY34" s="116"/>
+      <c r="BZ34" s="116"/>
+      <c r="CA34" s="116"/>
+      <c r="CB34" s="116"/>
+      <c r="CC34" s="116"/>
+      <c r="CD34" s="116"/>
+      <c r="CE34" s="116"/>
+      <c r="CF34" s="116"/>
+      <c r="CG34" s="116"/>
+      <c r="CH34" s="116"/>
+      <c r="CI34" s="116"/>
+      <c r="CJ34" s="116"/>
+      <c r="CK34" s="116"/>
+      <c r="CL34" s="116"/>
+      <c r="CM34" s="116"/>
+      <c r="CN34" s="116"/>
+      <c r="CO34" s="116"/>
+      <c r="CP34" s="116"/>
+      <c r="CQ34" s="116"/>
+      <c r="CR34" s="116"/>
+      <c r="CS34" s="116"/>
+      <c r="CT34" s="116"/>
+      <c r="CU34" s="116"/>
+      <c r="CV34" s="116"/>
+      <c r="CW34" s="116"/>
+      <c r="CX34" s="116"/>
+      <c r="CY34" s="116"/>
+      <c r="CZ34" s="116"/>
+      <c r="DA34" s="116"/>
+      <c r="DB34" s="116"/>
+      <c r="DC34" s="116"/>
+      <c r="DD34" s="116"/>
+      <c r="DE34" s="116"/>
+      <c r="DF34" s="116"/>
+      <c r="DG34" s="116"/>
+      <c r="DH34" s="116"/>
+      <c r="DI34" s="116"/>
+      <c r="DJ34" s="116"/>
+      <c r="DK34" s="116"/>
+      <c r="DL34" s="116"/>
+      <c r="DM34" s="116"/>
+      <c r="DN34" s="116"/>
+      <c r="DO34" s="116"/>
+      <c r="DP34" s="116"/>
+      <c r="DQ34" s="116"/>
+      <c r="DR34" s="116"/>
+      <c r="DS34" s="116"/>
+      <c r="DT34" s="116"/>
+      <c r="DU34" s="116"/>
+      <c r="DV34" s="116"/>
+      <c r="DW34" s="116"/>
+      <c r="DX34" s="116"/>
+      <c r="DY34" s="116"/>
+      <c r="DZ34" s="116"/>
+      <c r="EA34" s="116"/>
+      <c r="EB34" s="116"/>
+      <c r="EC34" s="116"/>
+      <c r="ED34" s="116"/>
+      <c r="EE34" s="116"/>
+      <c r="EF34" s="116"/>
+      <c r="EG34" s="116"/>
+      <c r="EH34" s="116"/>
+      <c r="EI34" s="116"/>
+      <c r="EJ34" s="116"/>
+      <c r="EK34" s="116"/>
+      <c r="EL34" s="116"/>
+      <c r="EM34" s="116"/>
+      <c r="EN34" s="116"/>
+      <c r="EO34" s="116"/>
+      <c r="EP34" s="116"/>
+      <c r="EQ34" s="116"/>
+      <c r="ER34" s="116"/>
+      <c r="ES34" s="116"/>
+      <c r="ET34" s="116"/>
+      <c r="EU34" s="116"/>
+      <c r="EV34" s="116"/>
+      <c r="EW34" s="116"/>
+      <c r="EX34" s="116"/>
+      <c r="EY34" s="116"/>
+      <c r="EZ34" s="116"/>
+      <c r="FA34" s="116"/>
+      <c r="FB34" s="116"/>
+      <c r="FC34" s="116"/>
+      <c r="FD34" s="116"/>
+      <c r="FE34" s="116"/>
+      <c r="FF34" s="116"/>
+      <c r="FG34" s="116"/>
+      <c r="FH34" s="116"/>
+      <c r="FI34" s="116"/>
+      <c r="FJ34" s="116"/>
+      <c r="FK34" s="116"/>
+      <c r="FL34" s="116"/>
+      <c r="FM34" s="116"/>
+      <c r="FN34" s="116"/>
+      <c r="FO34" s="116"/>
+      <c r="FP34" s="116"/>
+      <c r="FQ34" s="116"/>
+      <c r="FR34" s="116"/>
+      <c r="FS34" s="116"/>
+      <c r="FT34" s="116"/>
+      <c r="FU34" s="116"/>
+      <c r="FV34" s="116"/>
+      <c r="FW34" s="116"/>
+      <c r="FX34" s="116"/>
+      <c r="FY34" s="116"/>
+      <c r="FZ34" s="116"/>
+      <c r="GA34" s="116"/>
+      <c r="GB34" s="116"/>
+      <c r="GC34" s="116"/>
+      <c r="GD34" s="116"/>
+      <c r="GE34" s="116"/>
+      <c r="GF34" s="116"/>
+      <c r="GG34" s="116"/>
+      <c r="GH34" s="116"/>
+      <c r="GI34" s="116"/>
+      <c r="GJ34" s="116"/>
+      <c r="GK34" s="116"/>
+      <c r="GL34" s="116"/>
+      <c r="GM34" s="116"/>
+      <c r="GN34" s="116"/>
+      <c r="GO34" s="116"/>
+      <c r="GP34" s="116"/>
+      <c r="GQ34" s="116"/>
+      <c r="GR34" s="116"/>
+      <c r="GS34" s="116"/>
+      <c r="GT34" s="116"/>
+      <c r="GU34" s="116"/>
+      <c r="GV34" s="116"/>
+      <c r="GW34" s="116"/>
+      <c r="GX34" s="116"/>
+      <c r="GY34" s="116"/>
+      <c r="GZ34" s="116"/>
+      <c r="HA34" s="116"/>
+      <c r="HB34" s="116"/>
+      <c r="HC34" s="116"/>
+      <c r="HD34" s="116"/>
+      <c r="HE34" s="116"/>
+      <c r="HF34" s="116"/>
+      <c r="HG34" s="116"/>
+      <c r="HH34" s="116"/>
+      <c r="HI34" s="116"/>
+      <c r="HJ34" s="116"/>
+      <c r="HK34" s="116"/>
+      <c r="HL34" s="116"/>
+      <c r="HM34" s="116"/>
+      <c r="HN34" s="116"/>
+      <c r="HO34" s="116"/>
+      <c r="HP34" s="116"/>
+      <c r="HQ34" s="116"/>
+      <c r="HR34" s="116"/>
+      <c r="HS34" s="116"/>
+      <c r="HT34" s="116"/>
+      <c r="HU34" s="116"/>
+      <c r="HV34" s="116"/>
+      <c r="HW34" s="116"/>
+      <c r="HX34" s="116"/>
+      <c r="HY34" s="116"/>
+      <c r="HZ34" s="116"/>
+      <c r="IA34" s="116"/>
+      <c r="IB34" s="116"/>
+      <c r="IC34" s="116"/>
+      <c r="ID34" s="116"/>
+      <c r="IE34" s="116"/>
+      <c r="IF34" s="116"/>
+      <c r="IG34" s="116"/>
+      <c r="IH34" s="116"/>
+      <c r="II34" s="116"/>
+      <c r="IJ34" s="116"/>
+      <c r="IK34" s="116"/>
+      <c r="IL34" s="116"/>
+      <c r="IM34" s="116"/>
+      <c r="IN34" s="116"/>
+      <c r="IO34" s="116"/>
+      <c r="IP34" s="116"/>
+      <c r="IQ34" s="116"/>
+      <c r="IR34" s="116"/>
+    </row>
+    <row r="35" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="109" t="s">
         <v>293</v>
       </c>
-      <c r="B35" s="101" t="s">
+      <c r="B35" s="110" t="s">
         <v>279</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="82"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="62"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="104" t="s">
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="114"/>
+      <c r="L35" s="115"/>
+      <c r="M35" s="116"/>
+      <c r="N35" s="116"/>
+      <c r="O35" s="116"/>
+      <c r="P35" s="116"/>
+      <c r="Q35" s="116"/>
+      <c r="R35" s="116"/>
+      <c r="S35" s="116"/>
+      <c r="T35" s="116"/>
+      <c r="U35" s="116"/>
+      <c r="V35" s="116"/>
+      <c r="W35" s="116"/>
+      <c r="X35" s="116"/>
+      <c r="Y35" s="116"/>
+      <c r="Z35" s="116"/>
+      <c r="AA35" s="116"/>
+      <c r="AB35" s="116"/>
+      <c r="AC35" s="116"/>
+      <c r="AD35" s="116"/>
+      <c r="AE35" s="116"/>
+      <c r="AF35" s="116"/>
+      <c r="AG35" s="116"/>
+      <c r="AH35" s="116"/>
+      <c r="AI35" s="116"/>
+      <c r="AJ35" s="116"/>
+      <c r="AK35" s="116"/>
+      <c r="AL35" s="116"/>
+      <c r="AM35" s="116"/>
+      <c r="AN35" s="116"/>
+      <c r="AO35" s="116"/>
+      <c r="AP35" s="116"/>
+      <c r="AQ35" s="116"/>
+      <c r="AR35" s="116"/>
+      <c r="AS35" s="116"/>
+      <c r="AT35" s="116"/>
+      <c r="AU35" s="116"/>
+      <c r="AV35" s="116"/>
+      <c r="AW35" s="116"/>
+      <c r="AX35" s="116"/>
+      <c r="AY35" s="116"/>
+      <c r="AZ35" s="116"/>
+      <c r="BA35" s="116"/>
+      <c r="BB35" s="116"/>
+      <c r="BC35" s="116"/>
+      <c r="BD35" s="116"/>
+      <c r="BE35" s="116"/>
+      <c r="BF35" s="116"/>
+      <c r="BG35" s="116"/>
+      <c r="BH35" s="116"/>
+      <c r="BI35" s="116"/>
+      <c r="BJ35" s="116"/>
+      <c r="BK35" s="116"/>
+      <c r="BL35" s="116"/>
+      <c r="BM35" s="116"/>
+      <c r="BN35" s="116"/>
+      <c r="BO35" s="116"/>
+      <c r="BP35" s="116"/>
+      <c r="BQ35" s="116"/>
+      <c r="BR35" s="116"/>
+      <c r="BS35" s="116"/>
+      <c r="BT35" s="116"/>
+      <c r="BU35" s="116"/>
+      <c r="BV35" s="116"/>
+      <c r="BW35" s="116"/>
+      <c r="BX35" s="116"/>
+      <c r="BY35" s="116"/>
+      <c r="BZ35" s="116"/>
+      <c r="CA35" s="116"/>
+      <c r="CB35" s="116"/>
+      <c r="CC35" s="116"/>
+      <c r="CD35" s="116"/>
+      <c r="CE35" s="116"/>
+      <c r="CF35" s="116"/>
+      <c r="CG35" s="116"/>
+      <c r="CH35" s="116"/>
+      <c r="CI35" s="116"/>
+      <c r="CJ35" s="116"/>
+      <c r="CK35" s="116"/>
+      <c r="CL35" s="116"/>
+      <c r="CM35" s="116"/>
+      <c r="CN35" s="116"/>
+      <c r="CO35" s="116"/>
+      <c r="CP35" s="116"/>
+      <c r="CQ35" s="116"/>
+      <c r="CR35" s="116"/>
+      <c r="CS35" s="116"/>
+      <c r="CT35" s="116"/>
+      <c r="CU35" s="116"/>
+      <c r="CV35" s="116"/>
+      <c r="CW35" s="116"/>
+      <c r="CX35" s="116"/>
+      <c r="CY35" s="116"/>
+      <c r="CZ35" s="116"/>
+      <c r="DA35" s="116"/>
+      <c r="DB35" s="116"/>
+      <c r="DC35" s="116"/>
+      <c r="DD35" s="116"/>
+      <c r="DE35" s="116"/>
+      <c r="DF35" s="116"/>
+      <c r="DG35" s="116"/>
+      <c r="DH35" s="116"/>
+      <c r="DI35" s="116"/>
+      <c r="DJ35" s="116"/>
+      <c r="DK35" s="116"/>
+      <c r="DL35" s="116"/>
+      <c r="DM35" s="116"/>
+      <c r="DN35" s="116"/>
+      <c r="DO35" s="116"/>
+      <c r="DP35" s="116"/>
+      <c r="DQ35" s="116"/>
+      <c r="DR35" s="116"/>
+      <c r="DS35" s="116"/>
+      <c r="DT35" s="116"/>
+      <c r="DU35" s="116"/>
+      <c r="DV35" s="116"/>
+      <c r="DW35" s="116"/>
+      <c r="DX35" s="116"/>
+      <c r="DY35" s="116"/>
+      <c r="DZ35" s="116"/>
+      <c r="EA35" s="116"/>
+      <c r="EB35" s="116"/>
+      <c r="EC35" s="116"/>
+      <c r="ED35" s="116"/>
+      <c r="EE35" s="116"/>
+      <c r="EF35" s="116"/>
+      <c r="EG35" s="116"/>
+      <c r="EH35" s="116"/>
+      <c r="EI35" s="116"/>
+      <c r="EJ35" s="116"/>
+      <c r="EK35" s="116"/>
+      <c r="EL35" s="116"/>
+      <c r="EM35" s="116"/>
+      <c r="EN35" s="116"/>
+      <c r="EO35" s="116"/>
+      <c r="EP35" s="116"/>
+      <c r="EQ35" s="116"/>
+      <c r="ER35" s="116"/>
+      <c r="ES35" s="116"/>
+      <c r="ET35" s="116"/>
+      <c r="EU35" s="116"/>
+      <c r="EV35" s="116"/>
+      <c r="EW35" s="116"/>
+      <c r="EX35" s="116"/>
+      <c r="EY35" s="116"/>
+      <c r="EZ35" s="116"/>
+      <c r="FA35" s="116"/>
+      <c r="FB35" s="116"/>
+      <c r="FC35" s="116"/>
+      <c r="FD35" s="116"/>
+      <c r="FE35" s="116"/>
+      <c r="FF35" s="116"/>
+      <c r="FG35" s="116"/>
+      <c r="FH35" s="116"/>
+      <c r="FI35" s="116"/>
+      <c r="FJ35" s="116"/>
+      <c r="FK35" s="116"/>
+      <c r="FL35" s="116"/>
+      <c r="FM35" s="116"/>
+      <c r="FN35" s="116"/>
+      <c r="FO35" s="116"/>
+      <c r="FP35" s="116"/>
+      <c r="FQ35" s="116"/>
+      <c r="FR35" s="116"/>
+      <c r="FS35" s="116"/>
+      <c r="FT35" s="116"/>
+      <c r="FU35" s="116"/>
+      <c r="FV35" s="116"/>
+      <c r="FW35" s="116"/>
+      <c r="FX35" s="116"/>
+      <c r="FY35" s="116"/>
+      <c r="FZ35" s="116"/>
+      <c r="GA35" s="116"/>
+      <c r="GB35" s="116"/>
+      <c r="GC35" s="116"/>
+      <c r="GD35" s="116"/>
+      <c r="GE35" s="116"/>
+      <c r="GF35" s="116"/>
+      <c r="GG35" s="116"/>
+      <c r="GH35" s="116"/>
+      <c r="GI35" s="116"/>
+      <c r="GJ35" s="116"/>
+      <c r="GK35" s="116"/>
+      <c r="GL35" s="116"/>
+      <c r="GM35" s="116"/>
+      <c r="GN35" s="116"/>
+      <c r="GO35" s="116"/>
+      <c r="GP35" s="116"/>
+      <c r="GQ35" s="116"/>
+      <c r="GR35" s="116"/>
+      <c r="GS35" s="116"/>
+      <c r="GT35" s="116"/>
+      <c r="GU35" s="116"/>
+      <c r="GV35" s="116"/>
+      <c r="GW35" s="116"/>
+      <c r="GX35" s="116"/>
+      <c r="GY35" s="116"/>
+      <c r="GZ35" s="116"/>
+      <c r="HA35" s="116"/>
+      <c r="HB35" s="116"/>
+      <c r="HC35" s="116"/>
+      <c r="HD35" s="116"/>
+      <c r="HE35" s="116"/>
+      <c r="HF35" s="116"/>
+      <c r="HG35" s="116"/>
+      <c r="HH35" s="116"/>
+      <c r="HI35" s="116"/>
+      <c r="HJ35" s="116"/>
+      <c r="HK35" s="116"/>
+      <c r="HL35" s="116"/>
+      <c r="HM35" s="116"/>
+      <c r="HN35" s="116"/>
+      <c r="HO35" s="116"/>
+      <c r="HP35" s="116"/>
+      <c r="HQ35" s="116"/>
+      <c r="HR35" s="116"/>
+      <c r="HS35" s="116"/>
+      <c r="HT35" s="116"/>
+      <c r="HU35" s="116"/>
+      <c r="HV35" s="116"/>
+      <c r="HW35" s="116"/>
+      <c r="HX35" s="116"/>
+      <c r="HY35" s="116"/>
+      <c r="HZ35" s="116"/>
+      <c r="IA35" s="116"/>
+      <c r="IB35" s="116"/>
+      <c r="IC35" s="116"/>
+      <c r="ID35" s="116"/>
+      <c r="IE35" s="116"/>
+      <c r="IF35" s="116"/>
+      <c r="IG35" s="116"/>
+      <c r="IH35" s="116"/>
+      <c r="II35" s="116"/>
+      <c r="IJ35" s="116"/>
+      <c r="IK35" s="116"/>
+      <c r="IL35" s="116"/>
+      <c r="IM35" s="116"/>
+      <c r="IN35" s="116"/>
+      <c r="IO35" s="116"/>
+      <c r="IP35" s="116"/>
+      <c r="IQ35" s="116"/>
+      <c r="IR35" s="116"/>
+    </row>
+    <row r="36" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="114" t="s">
         <v>280</v>
       </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="111">
+      <c r="B36" s="111"/>
+      <c r="C36" s="119">
         <v>1</v>
       </c>
-      <c r="D36" s="112"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="62"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="104" t="s">
+      <c r="D36" s="120"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="122"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="123"/>
+      <c r="I36" s="111"/>
+      <c r="J36" s="124"/>
+      <c r="K36" s="114"/>
+      <c r="L36" s="115"/>
+      <c r="M36" s="116"/>
+      <c r="N36" s="116"/>
+      <c r="O36" s="116"/>
+      <c r="P36" s="116"/>
+      <c r="Q36" s="116"/>
+      <c r="R36" s="116"/>
+      <c r="S36" s="116"/>
+      <c r="T36" s="116"/>
+      <c r="U36" s="116"/>
+      <c r="V36" s="116"/>
+      <c r="W36" s="116"/>
+      <c r="X36" s="116"/>
+      <c r="Y36" s="116"/>
+      <c r="Z36" s="116"/>
+      <c r="AA36" s="116"/>
+      <c r="AB36" s="116"/>
+      <c r="AC36" s="116"/>
+      <c r="AD36" s="116"/>
+      <c r="AE36" s="116"/>
+      <c r="AF36" s="116"/>
+      <c r="AG36" s="116"/>
+      <c r="AH36" s="116"/>
+      <c r="AI36" s="116"/>
+      <c r="AJ36" s="116"/>
+      <c r="AK36" s="116"/>
+      <c r="AL36" s="116"/>
+      <c r="AM36" s="116"/>
+      <c r="AN36" s="116"/>
+      <c r="AO36" s="116"/>
+      <c r="AP36" s="116"/>
+      <c r="AQ36" s="116"/>
+      <c r="AR36" s="116"/>
+      <c r="AS36" s="116"/>
+      <c r="AT36" s="116"/>
+      <c r="AU36" s="116"/>
+      <c r="AV36" s="116"/>
+      <c r="AW36" s="116"/>
+      <c r="AX36" s="116"/>
+      <c r="AY36" s="116"/>
+      <c r="AZ36" s="116"/>
+      <c r="BA36" s="116"/>
+      <c r="BB36" s="116"/>
+      <c r="BC36" s="116"/>
+      <c r="BD36" s="116"/>
+      <c r="BE36" s="116"/>
+      <c r="BF36" s="116"/>
+      <c r="BG36" s="116"/>
+      <c r="BH36" s="116"/>
+      <c r="BI36" s="116"/>
+      <c r="BJ36" s="116"/>
+      <c r="BK36" s="116"/>
+      <c r="BL36" s="116"/>
+      <c r="BM36" s="116"/>
+      <c r="BN36" s="116"/>
+      <c r="BO36" s="116"/>
+      <c r="BP36" s="116"/>
+      <c r="BQ36" s="116"/>
+      <c r="BR36" s="116"/>
+      <c r="BS36" s="116"/>
+      <c r="BT36" s="116"/>
+      <c r="BU36" s="116"/>
+      <c r="BV36" s="116"/>
+      <c r="BW36" s="116"/>
+      <c r="BX36" s="116"/>
+      <c r="BY36" s="116"/>
+      <c r="BZ36" s="116"/>
+      <c r="CA36" s="116"/>
+      <c r="CB36" s="116"/>
+      <c r="CC36" s="116"/>
+      <c r="CD36" s="116"/>
+      <c r="CE36" s="116"/>
+      <c r="CF36" s="116"/>
+      <c r="CG36" s="116"/>
+      <c r="CH36" s="116"/>
+      <c r="CI36" s="116"/>
+      <c r="CJ36" s="116"/>
+      <c r="CK36" s="116"/>
+      <c r="CL36" s="116"/>
+      <c r="CM36" s="116"/>
+      <c r="CN36" s="116"/>
+      <c r="CO36" s="116"/>
+      <c r="CP36" s="116"/>
+      <c r="CQ36" s="116"/>
+      <c r="CR36" s="116"/>
+      <c r="CS36" s="116"/>
+      <c r="CT36" s="116"/>
+      <c r="CU36" s="116"/>
+      <c r="CV36" s="116"/>
+      <c r="CW36" s="116"/>
+      <c r="CX36" s="116"/>
+      <c r="CY36" s="116"/>
+      <c r="CZ36" s="116"/>
+      <c r="DA36" s="116"/>
+      <c r="DB36" s="116"/>
+      <c r="DC36" s="116"/>
+      <c r="DD36" s="116"/>
+      <c r="DE36" s="116"/>
+      <c r="DF36" s="116"/>
+      <c r="DG36" s="116"/>
+      <c r="DH36" s="116"/>
+      <c r="DI36" s="116"/>
+      <c r="DJ36" s="116"/>
+      <c r="DK36" s="116"/>
+      <c r="DL36" s="116"/>
+      <c r="DM36" s="116"/>
+      <c r="DN36" s="116"/>
+      <c r="DO36" s="116"/>
+      <c r="DP36" s="116"/>
+      <c r="DQ36" s="116"/>
+      <c r="DR36" s="116"/>
+      <c r="DS36" s="116"/>
+      <c r="DT36" s="116"/>
+      <c r="DU36" s="116"/>
+      <c r="DV36" s="116"/>
+      <c r="DW36" s="116"/>
+      <c r="DX36" s="116"/>
+      <c r="DY36" s="116"/>
+      <c r="DZ36" s="116"/>
+      <c r="EA36" s="116"/>
+      <c r="EB36" s="116"/>
+      <c r="EC36" s="116"/>
+      <c r="ED36" s="116"/>
+      <c r="EE36" s="116"/>
+      <c r="EF36" s="116"/>
+      <c r="EG36" s="116"/>
+      <c r="EH36" s="116"/>
+      <c r="EI36" s="116"/>
+      <c r="EJ36" s="116"/>
+      <c r="EK36" s="116"/>
+      <c r="EL36" s="116"/>
+      <c r="EM36" s="116"/>
+      <c r="EN36" s="116"/>
+      <c r="EO36" s="116"/>
+      <c r="EP36" s="116"/>
+      <c r="EQ36" s="116"/>
+      <c r="ER36" s="116"/>
+      <c r="ES36" s="116"/>
+      <c r="ET36" s="116"/>
+      <c r="EU36" s="116"/>
+      <c r="EV36" s="116"/>
+      <c r="EW36" s="116"/>
+      <c r="EX36" s="116"/>
+      <c r="EY36" s="116"/>
+      <c r="EZ36" s="116"/>
+      <c r="FA36" s="116"/>
+      <c r="FB36" s="116"/>
+      <c r="FC36" s="116"/>
+      <c r="FD36" s="116"/>
+      <c r="FE36" s="116"/>
+      <c r="FF36" s="116"/>
+      <c r="FG36" s="116"/>
+      <c r="FH36" s="116"/>
+      <c r="FI36" s="116"/>
+      <c r="FJ36" s="116"/>
+      <c r="FK36" s="116"/>
+      <c r="FL36" s="116"/>
+      <c r="FM36" s="116"/>
+      <c r="FN36" s="116"/>
+      <c r="FO36" s="116"/>
+      <c r="FP36" s="116"/>
+      <c r="FQ36" s="116"/>
+      <c r="FR36" s="116"/>
+      <c r="FS36" s="116"/>
+      <c r="FT36" s="116"/>
+      <c r="FU36" s="116"/>
+      <c r="FV36" s="116"/>
+      <c r="FW36" s="116"/>
+      <c r="FX36" s="116"/>
+      <c r="FY36" s="116"/>
+      <c r="FZ36" s="116"/>
+      <c r="GA36" s="116"/>
+      <c r="GB36" s="116"/>
+      <c r="GC36" s="116"/>
+      <c r="GD36" s="116"/>
+      <c r="GE36" s="116"/>
+      <c r="GF36" s="116"/>
+      <c r="GG36" s="116"/>
+      <c r="GH36" s="116"/>
+      <c r="GI36" s="116"/>
+      <c r="GJ36" s="116"/>
+      <c r="GK36" s="116"/>
+      <c r="GL36" s="116"/>
+      <c r="GM36" s="116"/>
+      <c r="GN36" s="116"/>
+      <c r="GO36" s="116"/>
+      <c r="GP36" s="116"/>
+      <c r="GQ36" s="116"/>
+      <c r="GR36" s="116"/>
+      <c r="GS36" s="116"/>
+      <c r="GT36" s="116"/>
+      <c r="GU36" s="116"/>
+      <c r="GV36" s="116"/>
+      <c r="GW36" s="116"/>
+      <c r="GX36" s="116"/>
+      <c r="GY36" s="116"/>
+      <c r="GZ36" s="116"/>
+      <c r="HA36" s="116"/>
+      <c r="HB36" s="116"/>
+      <c r="HC36" s="116"/>
+      <c r="HD36" s="116"/>
+      <c r="HE36" s="116"/>
+      <c r="HF36" s="116"/>
+      <c r="HG36" s="116"/>
+      <c r="HH36" s="116"/>
+      <c r="HI36" s="116"/>
+      <c r="HJ36" s="116"/>
+      <c r="HK36" s="116"/>
+      <c r="HL36" s="116"/>
+      <c r="HM36" s="116"/>
+      <c r="HN36" s="116"/>
+      <c r="HO36" s="116"/>
+      <c r="HP36" s="116"/>
+      <c r="HQ36" s="116"/>
+      <c r="HR36" s="116"/>
+      <c r="HS36" s="116"/>
+      <c r="HT36" s="116"/>
+      <c r="HU36" s="116"/>
+      <c r="HV36" s="116"/>
+      <c r="HW36" s="116"/>
+      <c r="HX36" s="116"/>
+      <c r="HY36" s="116"/>
+      <c r="HZ36" s="116"/>
+      <c r="IA36" s="116"/>
+      <c r="IB36" s="116"/>
+      <c r="IC36" s="116"/>
+      <c r="ID36" s="116"/>
+      <c r="IE36" s="116"/>
+      <c r="IF36" s="116"/>
+      <c r="IG36" s="116"/>
+      <c r="IH36" s="116"/>
+      <c r="II36" s="116"/>
+      <c r="IJ36" s="116"/>
+      <c r="IK36" s="116"/>
+      <c r="IL36" s="116"/>
+      <c r="IM36" s="116"/>
+      <c r="IN36" s="116"/>
+      <c r="IO36" s="116"/>
+      <c r="IP36" s="116"/>
+      <c r="IQ36" s="116"/>
+      <c r="IR36" s="116"/>
+    </row>
+    <row r="37" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="114" t="s">
         <v>281</v>
       </c>
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="111" t="s">
         <v>282</v>
       </c>
-      <c r="C37" s="111">
+      <c r="C37" s="119">
         <v>50000</v>
       </c>
-      <c r="D37" s="112"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="106"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="62"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="104" t="s">
+      <c r="D37" s="120"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="123"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="124"/>
+      <c r="K37" s="114"/>
+      <c r="L37" s="115"/>
+      <c r="M37" s="116"/>
+      <c r="N37" s="116"/>
+      <c r="O37" s="116"/>
+      <c r="P37" s="116"/>
+      <c r="Q37" s="116"/>
+      <c r="R37" s="116"/>
+      <c r="S37" s="116"/>
+      <c r="T37" s="116"/>
+      <c r="U37" s="116"/>
+      <c r="V37" s="116"/>
+      <c r="W37" s="116"/>
+      <c r="X37" s="116"/>
+      <c r="Y37" s="116"/>
+      <c r="Z37" s="116"/>
+      <c r="AA37" s="116"/>
+      <c r="AB37" s="116"/>
+      <c r="AC37" s="116"/>
+      <c r="AD37" s="116"/>
+      <c r="AE37" s="116"/>
+      <c r="AF37" s="116"/>
+      <c r="AG37" s="116"/>
+      <c r="AH37" s="116"/>
+      <c r="AI37" s="116"/>
+      <c r="AJ37" s="116"/>
+      <c r="AK37" s="116"/>
+      <c r="AL37" s="116"/>
+      <c r="AM37" s="116"/>
+      <c r="AN37" s="116"/>
+      <c r="AO37" s="116"/>
+      <c r="AP37" s="116"/>
+      <c r="AQ37" s="116"/>
+      <c r="AR37" s="116"/>
+      <c r="AS37" s="116"/>
+      <c r="AT37" s="116"/>
+      <c r="AU37" s="116"/>
+      <c r="AV37" s="116"/>
+      <c r="AW37" s="116"/>
+      <c r="AX37" s="116"/>
+      <c r="AY37" s="116"/>
+      <c r="AZ37" s="116"/>
+      <c r="BA37" s="116"/>
+      <c r="BB37" s="116"/>
+      <c r="BC37" s="116"/>
+      <c r="BD37" s="116"/>
+      <c r="BE37" s="116"/>
+      <c r="BF37" s="116"/>
+      <c r="BG37" s="116"/>
+      <c r="BH37" s="116"/>
+      <c r="BI37" s="116"/>
+      <c r="BJ37" s="116"/>
+      <c r="BK37" s="116"/>
+      <c r="BL37" s="116"/>
+      <c r="BM37" s="116"/>
+      <c r="BN37" s="116"/>
+      <c r="BO37" s="116"/>
+      <c r="BP37" s="116"/>
+      <c r="BQ37" s="116"/>
+      <c r="BR37" s="116"/>
+      <c r="BS37" s="116"/>
+      <c r="BT37" s="116"/>
+      <c r="BU37" s="116"/>
+      <c r="BV37" s="116"/>
+      <c r="BW37" s="116"/>
+      <c r="BX37" s="116"/>
+      <c r="BY37" s="116"/>
+      <c r="BZ37" s="116"/>
+      <c r="CA37" s="116"/>
+      <c r="CB37" s="116"/>
+      <c r="CC37" s="116"/>
+      <c r="CD37" s="116"/>
+      <c r="CE37" s="116"/>
+      <c r="CF37" s="116"/>
+      <c r="CG37" s="116"/>
+      <c r="CH37" s="116"/>
+      <c r="CI37" s="116"/>
+      <c r="CJ37" s="116"/>
+      <c r="CK37" s="116"/>
+      <c r="CL37" s="116"/>
+      <c r="CM37" s="116"/>
+      <c r="CN37" s="116"/>
+      <c r="CO37" s="116"/>
+      <c r="CP37" s="116"/>
+      <c r="CQ37" s="116"/>
+      <c r="CR37" s="116"/>
+      <c r="CS37" s="116"/>
+      <c r="CT37" s="116"/>
+      <c r="CU37" s="116"/>
+      <c r="CV37" s="116"/>
+      <c r="CW37" s="116"/>
+      <c r="CX37" s="116"/>
+      <c r="CY37" s="116"/>
+      <c r="CZ37" s="116"/>
+      <c r="DA37" s="116"/>
+      <c r="DB37" s="116"/>
+      <c r="DC37" s="116"/>
+      <c r="DD37" s="116"/>
+      <c r="DE37" s="116"/>
+      <c r="DF37" s="116"/>
+      <c r="DG37" s="116"/>
+      <c r="DH37" s="116"/>
+      <c r="DI37" s="116"/>
+      <c r="DJ37" s="116"/>
+      <c r="DK37" s="116"/>
+      <c r="DL37" s="116"/>
+      <c r="DM37" s="116"/>
+      <c r="DN37" s="116"/>
+      <c r="DO37" s="116"/>
+      <c r="DP37" s="116"/>
+      <c r="DQ37" s="116"/>
+      <c r="DR37" s="116"/>
+      <c r="DS37" s="116"/>
+      <c r="DT37" s="116"/>
+      <c r="DU37" s="116"/>
+      <c r="DV37" s="116"/>
+      <c r="DW37" s="116"/>
+      <c r="DX37" s="116"/>
+      <c r="DY37" s="116"/>
+      <c r="DZ37" s="116"/>
+      <c r="EA37" s="116"/>
+      <c r="EB37" s="116"/>
+      <c r="EC37" s="116"/>
+      <c r="ED37" s="116"/>
+      <c r="EE37" s="116"/>
+      <c r="EF37" s="116"/>
+      <c r="EG37" s="116"/>
+      <c r="EH37" s="116"/>
+      <c r="EI37" s="116"/>
+      <c r="EJ37" s="116"/>
+      <c r="EK37" s="116"/>
+      <c r="EL37" s="116"/>
+      <c r="EM37" s="116"/>
+      <c r="EN37" s="116"/>
+      <c r="EO37" s="116"/>
+      <c r="EP37" s="116"/>
+      <c r="EQ37" s="116"/>
+      <c r="ER37" s="116"/>
+      <c r="ES37" s="116"/>
+      <c r="ET37" s="116"/>
+      <c r="EU37" s="116"/>
+      <c r="EV37" s="116"/>
+      <c r="EW37" s="116"/>
+      <c r="EX37" s="116"/>
+      <c r="EY37" s="116"/>
+      <c r="EZ37" s="116"/>
+      <c r="FA37" s="116"/>
+      <c r="FB37" s="116"/>
+      <c r="FC37" s="116"/>
+      <c r="FD37" s="116"/>
+      <c r="FE37" s="116"/>
+      <c r="FF37" s="116"/>
+      <c r="FG37" s="116"/>
+      <c r="FH37" s="116"/>
+      <c r="FI37" s="116"/>
+      <c r="FJ37" s="116"/>
+      <c r="FK37" s="116"/>
+      <c r="FL37" s="116"/>
+      <c r="FM37" s="116"/>
+      <c r="FN37" s="116"/>
+      <c r="FO37" s="116"/>
+      <c r="FP37" s="116"/>
+      <c r="FQ37" s="116"/>
+      <c r="FR37" s="116"/>
+      <c r="FS37" s="116"/>
+      <c r="FT37" s="116"/>
+      <c r="FU37" s="116"/>
+      <c r="FV37" s="116"/>
+      <c r="FW37" s="116"/>
+      <c r="FX37" s="116"/>
+      <c r="FY37" s="116"/>
+      <c r="FZ37" s="116"/>
+      <c r="GA37" s="116"/>
+      <c r="GB37" s="116"/>
+      <c r="GC37" s="116"/>
+      <c r="GD37" s="116"/>
+      <c r="GE37" s="116"/>
+      <c r="GF37" s="116"/>
+      <c r="GG37" s="116"/>
+      <c r="GH37" s="116"/>
+      <c r="GI37" s="116"/>
+      <c r="GJ37" s="116"/>
+      <c r="GK37" s="116"/>
+      <c r="GL37" s="116"/>
+      <c r="GM37" s="116"/>
+      <c r="GN37" s="116"/>
+      <c r="GO37" s="116"/>
+      <c r="GP37" s="116"/>
+      <c r="GQ37" s="116"/>
+      <c r="GR37" s="116"/>
+      <c r="GS37" s="116"/>
+      <c r="GT37" s="116"/>
+      <c r="GU37" s="116"/>
+      <c r="GV37" s="116"/>
+      <c r="GW37" s="116"/>
+      <c r="GX37" s="116"/>
+      <c r="GY37" s="116"/>
+      <c r="GZ37" s="116"/>
+      <c r="HA37" s="116"/>
+      <c r="HB37" s="116"/>
+      <c r="HC37" s="116"/>
+      <c r="HD37" s="116"/>
+      <c r="HE37" s="116"/>
+      <c r="HF37" s="116"/>
+      <c r="HG37" s="116"/>
+      <c r="HH37" s="116"/>
+      <c r="HI37" s="116"/>
+      <c r="HJ37" s="116"/>
+      <c r="HK37" s="116"/>
+      <c r="HL37" s="116"/>
+      <c r="HM37" s="116"/>
+      <c r="HN37" s="116"/>
+      <c r="HO37" s="116"/>
+      <c r="HP37" s="116"/>
+      <c r="HQ37" s="116"/>
+      <c r="HR37" s="116"/>
+      <c r="HS37" s="116"/>
+      <c r="HT37" s="116"/>
+      <c r="HU37" s="116"/>
+      <c r="HV37" s="116"/>
+      <c r="HW37" s="116"/>
+      <c r="HX37" s="116"/>
+      <c r="HY37" s="116"/>
+      <c r="HZ37" s="116"/>
+      <c r="IA37" s="116"/>
+      <c r="IB37" s="116"/>
+      <c r="IC37" s="116"/>
+      <c r="ID37" s="116"/>
+      <c r="IE37" s="116"/>
+      <c r="IF37" s="116"/>
+      <c r="IG37" s="116"/>
+      <c r="IH37" s="116"/>
+      <c r="II37" s="116"/>
+      <c r="IJ37" s="116"/>
+      <c r="IK37" s="116"/>
+      <c r="IL37" s="116"/>
+      <c r="IM37" s="116"/>
+      <c r="IN37" s="116"/>
+      <c r="IO37" s="116"/>
+      <c r="IP37" s="116"/>
+      <c r="IQ37" s="116"/>
+      <c r="IR37" s="116"/>
+    </row>
+    <row r="38" spans="1:252" s="117" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="114" t="s">
         <v>260</v>
       </c>
-      <c r="B38" s="107" t="s">
+      <c r="B38" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="C38" s="111">
+      <c r="C38" s="119">
         <v>250000</v>
       </c>
-      <c r="D38" s="112"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="62"/>
-    </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="120"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="122"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="124"/>
+      <c r="K38" s="114"/>
+      <c r="L38" s="115"/>
+      <c r="M38" s="116"/>
+      <c r="N38" s="116"/>
+      <c r="O38" s="116"/>
+      <c r="P38" s="116"/>
+      <c r="Q38" s="116"/>
+      <c r="R38" s="116"/>
+      <c r="S38" s="116"/>
+      <c r="T38" s="116"/>
+      <c r="U38" s="116"/>
+      <c r="V38" s="116"/>
+      <c r="W38" s="116"/>
+      <c r="X38" s="116"/>
+      <c r="Y38" s="116"/>
+      <c r="Z38" s="116"/>
+      <c r="AA38" s="116"/>
+      <c r="AB38" s="116"/>
+      <c r="AC38" s="116"/>
+      <c r="AD38" s="116"/>
+      <c r="AE38" s="116"/>
+      <c r="AF38" s="116"/>
+      <c r="AG38" s="116"/>
+      <c r="AH38" s="116"/>
+      <c r="AI38" s="116"/>
+      <c r="AJ38" s="116"/>
+      <c r="AK38" s="116"/>
+      <c r="AL38" s="116"/>
+      <c r="AM38" s="116"/>
+      <c r="AN38" s="116"/>
+      <c r="AO38" s="116"/>
+      <c r="AP38" s="116"/>
+      <c r="AQ38" s="116"/>
+      <c r="AR38" s="116"/>
+      <c r="AS38" s="116"/>
+      <c r="AT38" s="116"/>
+      <c r="AU38" s="116"/>
+      <c r="AV38" s="116"/>
+      <c r="AW38" s="116"/>
+      <c r="AX38" s="116"/>
+      <c r="AY38" s="116"/>
+      <c r="AZ38" s="116"/>
+      <c r="BA38" s="116"/>
+      <c r="BB38" s="116"/>
+      <c r="BC38" s="116"/>
+      <c r="BD38" s="116"/>
+      <c r="BE38" s="116"/>
+      <c r="BF38" s="116"/>
+      <c r="BG38" s="116"/>
+      <c r="BH38" s="116"/>
+      <c r="BI38" s="116"/>
+      <c r="BJ38" s="116"/>
+      <c r="BK38" s="116"/>
+      <c r="BL38" s="116"/>
+      <c r="BM38" s="116"/>
+      <c r="BN38" s="116"/>
+      <c r="BO38" s="116"/>
+      <c r="BP38" s="116"/>
+      <c r="BQ38" s="116"/>
+      <c r="BR38" s="116"/>
+      <c r="BS38" s="116"/>
+      <c r="BT38" s="116"/>
+      <c r="BU38" s="116"/>
+      <c r="BV38" s="116"/>
+      <c r="BW38" s="116"/>
+      <c r="BX38" s="116"/>
+      <c r="BY38" s="116"/>
+      <c r="BZ38" s="116"/>
+      <c r="CA38" s="116"/>
+      <c r="CB38" s="116"/>
+      <c r="CC38" s="116"/>
+      <c r="CD38" s="116"/>
+      <c r="CE38" s="116"/>
+      <c r="CF38" s="116"/>
+      <c r="CG38" s="116"/>
+      <c r="CH38" s="116"/>
+      <c r="CI38" s="116"/>
+      <c r="CJ38" s="116"/>
+      <c r="CK38" s="116"/>
+      <c r="CL38" s="116"/>
+      <c r="CM38" s="116"/>
+      <c r="CN38" s="116"/>
+      <c r="CO38" s="116"/>
+      <c r="CP38" s="116"/>
+      <c r="CQ38" s="116"/>
+      <c r="CR38" s="116"/>
+      <c r="CS38" s="116"/>
+      <c r="CT38" s="116"/>
+      <c r="CU38" s="116"/>
+      <c r="CV38" s="116"/>
+      <c r="CW38" s="116"/>
+      <c r="CX38" s="116"/>
+      <c r="CY38" s="116"/>
+      <c r="CZ38" s="116"/>
+      <c r="DA38" s="116"/>
+      <c r="DB38" s="116"/>
+      <c r="DC38" s="116"/>
+      <c r="DD38" s="116"/>
+      <c r="DE38" s="116"/>
+      <c r="DF38" s="116"/>
+      <c r="DG38" s="116"/>
+      <c r="DH38" s="116"/>
+      <c r="DI38" s="116"/>
+      <c r="DJ38" s="116"/>
+      <c r="DK38" s="116"/>
+      <c r="DL38" s="116"/>
+      <c r="DM38" s="116"/>
+      <c r="DN38" s="116"/>
+      <c r="DO38" s="116"/>
+      <c r="DP38" s="116"/>
+      <c r="DQ38" s="116"/>
+      <c r="DR38" s="116"/>
+      <c r="DS38" s="116"/>
+      <c r="DT38" s="116"/>
+      <c r="DU38" s="116"/>
+      <c r="DV38" s="116"/>
+      <c r="DW38" s="116"/>
+      <c r="DX38" s="116"/>
+      <c r="DY38" s="116"/>
+      <c r="DZ38" s="116"/>
+      <c r="EA38" s="116"/>
+      <c r="EB38" s="116"/>
+      <c r="EC38" s="116"/>
+      <c r="ED38" s="116"/>
+      <c r="EE38" s="116"/>
+      <c r="EF38" s="116"/>
+      <c r="EG38" s="116"/>
+      <c r="EH38" s="116"/>
+      <c r="EI38" s="116"/>
+      <c r="EJ38" s="116"/>
+      <c r="EK38" s="116"/>
+      <c r="EL38" s="116"/>
+      <c r="EM38" s="116"/>
+      <c r="EN38" s="116"/>
+      <c r="EO38" s="116"/>
+      <c r="EP38" s="116"/>
+      <c r="EQ38" s="116"/>
+      <c r="ER38" s="116"/>
+      <c r="ES38" s="116"/>
+      <c r="ET38" s="116"/>
+      <c r="EU38" s="116"/>
+      <c r="EV38" s="116"/>
+      <c r="EW38" s="116"/>
+      <c r="EX38" s="116"/>
+      <c r="EY38" s="116"/>
+      <c r="EZ38" s="116"/>
+      <c r="FA38" s="116"/>
+      <c r="FB38" s="116"/>
+      <c r="FC38" s="116"/>
+      <c r="FD38" s="116"/>
+      <c r="FE38" s="116"/>
+      <c r="FF38" s="116"/>
+      <c r="FG38" s="116"/>
+      <c r="FH38" s="116"/>
+      <c r="FI38" s="116"/>
+      <c r="FJ38" s="116"/>
+      <c r="FK38" s="116"/>
+      <c r="FL38" s="116"/>
+      <c r="FM38" s="116"/>
+      <c r="FN38" s="116"/>
+      <c r="FO38" s="116"/>
+      <c r="FP38" s="116"/>
+      <c r="FQ38" s="116"/>
+      <c r="FR38" s="116"/>
+      <c r="FS38" s="116"/>
+      <c r="FT38" s="116"/>
+      <c r="FU38" s="116"/>
+      <c r="FV38" s="116"/>
+      <c r="FW38" s="116"/>
+      <c r="FX38" s="116"/>
+      <c r="FY38" s="116"/>
+      <c r="FZ38" s="116"/>
+      <c r="GA38" s="116"/>
+      <c r="GB38" s="116"/>
+      <c r="GC38" s="116"/>
+      <c r="GD38" s="116"/>
+      <c r="GE38" s="116"/>
+      <c r="GF38" s="116"/>
+      <c r="GG38" s="116"/>
+      <c r="GH38" s="116"/>
+      <c r="GI38" s="116"/>
+      <c r="GJ38" s="116"/>
+      <c r="GK38" s="116"/>
+      <c r="GL38" s="116"/>
+      <c r="GM38" s="116"/>
+      <c r="GN38" s="116"/>
+      <c r="GO38" s="116"/>
+      <c r="GP38" s="116"/>
+      <c r="GQ38" s="116"/>
+      <c r="GR38" s="116"/>
+      <c r="GS38" s="116"/>
+      <c r="GT38" s="116"/>
+      <c r="GU38" s="116"/>
+      <c r="GV38" s="116"/>
+      <c r="GW38" s="116"/>
+      <c r="GX38" s="116"/>
+      <c r="GY38" s="116"/>
+      <c r="GZ38" s="116"/>
+      <c r="HA38" s="116"/>
+      <c r="HB38" s="116"/>
+      <c r="HC38" s="116"/>
+      <c r="HD38" s="116"/>
+      <c r="HE38" s="116"/>
+      <c r="HF38" s="116"/>
+      <c r="HG38" s="116"/>
+      <c r="HH38" s="116"/>
+      <c r="HI38" s="116"/>
+      <c r="HJ38" s="116"/>
+      <c r="HK38" s="116"/>
+      <c r="HL38" s="116"/>
+      <c r="HM38" s="116"/>
+      <c r="HN38" s="116"/>
+      <c r="HO38" s="116"/>
+      <c r="HP38" s="116"/>
+      <c r="HQ38" s="116"/>
+      <c r="HR38" s="116"/>
+      <c r="HS38" s="116"/>
+      <c r="HT38" s="116"/>
+      <c r="HU38" s="116"/>
+      <c r="HV38" s="116"/>
+      <c r="HW38" s="116"/>
+      <c r="HX38" s="116"/>
+      <c r="HY38" s="116"/>
+      <c r="HZ38" s="116"/>
+      <c r="IA38" s="116"/>
+      <c r="IB38" s="116"/>
+      <c r="IC38" s="116"/>
+      <c r="ID38" s="116"/>
+      <c r="IE38" s="116"/>
+      <c r="IF38" s="116"/>
+      <c r="IG38" s="116"/>
+      <c r="IH38" s="116"/>
+      <c r="II38" s="116"/>
+      <c r="IJ38" s="116"/>
+      <c r="IK38" s="116"/>
+      <c r="IL38" s="116"/>
+      <c r="IM38" s="116"/>
+      <c r="IN38" s="116"/>
+      <c r="IO38" s="116"/>
+      <c r="IP38" s="116"/>
+      <c r="IQ38" s="116"/>
+      <c r="IR38" s="116"/>
+    </row>
+    <row r="39" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="106" t="s">
         <v>251</v>
       </c>
       <c r="C39" s="105"/>
@@ -10542,11 +12011,11 @@
       <c r="K39" s="73"/>
       <c r="L39" s="62"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="104" t="s">
         <v>260</v>
       </c>
-      <c r="B40" s="107" t="s">
+      <c r="B40" s="106" t="s">
         <v>283</v>
       </c>
       <c r="C40" s="105"/>
@@ -10562,7 +12031,7 @@
       <c r="K40" s="73"/>
       <c r="L40" s="62"/>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="74" t="s">
         <v>262</v>
       </c>
@@ -10578,7 +12047,7 @@
       <c r="K41" s="73"/>
       <c r="L41" s="62"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="78" t="s">
         <v>263</v>
       </c>
@@ -10608,7 +12077,7 @@
       <c r="K42" s="73"/>
       <c r="L42" s="62"/>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="73"/>
       <c r="B43" s="61"/>
       <c r="C43" s="83"/>
@@ -10622,7 +12091,7 @@
       <c r="K43" s="73"/>
       <c r="L43" s="62"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="74" t="s">
         <v>265</v>
       </c>
@@ -10640,7 +12109,7 @@
       <c r="K44" s="73"/>
       <c r="L44" s="62"/>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="78" t="s">
         <v>267</v>
       </c>
@@ -10679,7 +12148,7 @@
       <c r="K45" s="73"/>
       <c r="L45" s="62"/>
     </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="103" t="s">
         <v>284</v>
       </c>
@@ -10687,27 +12156,27 @@
         <v>269</v>
       </c>
       <c r="C46" s="94">
-        <f>MAX(C45-IF(C34=2,C33*C31,IF(C34=1,C45*C33,C33)),0)</f>
+        <f t="shared" ref="C46:H46" si="1">MAX(C45-IF(C34=2,C33*C31,IF(C34=1,C45*C33,C33)),0)</f>
         <v>990000</v>
       </c>
       <c r="D46" s="94">
-        <f>MAX(D45-IF(D34=2,D33*D31,IF(D34=1,D45*D33,D33)),0)</f>
+        <f t="shared" si="1"/>
         <v>990000</v>
       </c>
       <c r="E46" s="94">
-        <f>MAX(E45-IF(E34=2,E33*E31,IF(E34=1,E45*E33,E33)),0)</f>
+        <f t="shared" si="1"/>
         <v>950000</v>
       </c>
       <c r="F46" s="94">
-        <f>MAX(F45-IF(F34=2,F33*F31,IF(F34=1,F45*F33,F33)),0)</f>
+        <f t="shared" si="1"/>
         <v>1985000</v>
       </c>
       <c r="G46" s="94">
-        <f>MAX(G45-IF(G34=2,G33*G31,IF(G34=1,G45*G33,G33)),0)</f>
+        <f t="shared" si="1"/>
         <v>1990000</v>
       </c>
       <c r="H46" s="94">
-        <f>MAX(H45-IF(H34=2,H33*H31,IF(H34=1,H45*H33,H33)),0)</f>
+        <f t="shared" si="1"/>
         <v>1800000</v>
       </c>
       <c r="I46" s="61"/>
@@ -10718,7 +12187,7 @@
       <c r="K46" s="73"/>
       <c r="L46" s="62"/>
     </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="103" t="s">
         <v>285</v>
       </c>
@@ -10728,23 +12197,23 @@
         <v>10000</v>
       </c>
       <c r="D47" s="94">
-        <f t="shared" ref="D47:H47" si="1">D45-D46</f>
+        <f t="shared" ref="D47:H47" si="2">D45-D46</f>
         <v>10000</v>
       </c>
       <c r="E47" s="94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50000</v>
       </c>
       <c r="F47" s="94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15000</v>
       </c>
       <c r="G47" s="94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
       <c r="H47" s="94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200000</v>
       </c>
       <c r="I47" s="61"/>
@@ -10755,22 +12224,22 @@
       <c r="K47" s="73"/>
       <c r="L47" s="62"/>
     </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:252" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="103" t="s">
         <v>286</v>
       </c>
       <c r="B48" s="66"/>
-      <c r="C48" s="109">
+      <c r="C48" s="108">
         <f>MIN(MAX(C37,SUM(C47:E47)),SUM(C45:E45))</f>
         <v>70000</v>
       </c>
-      <c r="D48" s="109"/>
-      <c r="E48" s="109"/>
-      <c r="F48" s="109">
-        <v>0</v>
-      </c>
-      <c r="G48" s="109"/>
-      <c r="H48" s="109"/>
+      <c r="D48" s="108"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108">
+        <v>0</v>
+      </c>
+      <c r="G48" s="108"/>
+      <c r="H48" s="108"/>
       <c r="I48" s="61"/>
       <c r="J48" s="91"/>
       <c r="K48" s="73"/>
@@ -10781,18 +12250,18 @@
         <v>287</v>
       </c>
       <c r="B49" s="66"/>
-      <c r="C49" s="109">
+      <c r="C49" s="108">
         <f>MIN(C38,MAX(SUM(C45:E45)-C48,0))</f>
         <v>250000</v>
       </c>
-      <c r="D49" s="109"/>
-      <c r="E49" s="109"/>
-      <c r="F49" s="109">
+      <c r="D49" s="108"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108">
         <f>SUM(F46:H46)</f>
         <v>5775000</v>
       </c>
-      <c r="G49" s="109"/>
-      <c r="H49" s="109"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="108"/>
       <c r="I49" s="61"/>
       <c r="J49" s="91">
         <f>SUM(C49:H49)</f>
@@ -10861,27 +12330,27 @@
       </c>
       <c r="B53" s="61"/>
       <c r="C53" s="94">
-        <f t="shared" ref="C53:H53" si="2">$J$51*C45/SUM($C$45:$H$45)</f>
+        <f t="shared" ref="C53:H53" si="3">$J$51*C45/SUM($C$45:$H$45)</f>
         <v>166666.66666666666</v>
       </c>
       <c r="D53" s="94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166666.66666666666</v>
       </c>
       <c r="E53" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166666.66666666666</v>
       </c>
       <c r="F53" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>333333.33333333331</v>
       </c>
       <c r="G53" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>333333.33333333331</v>
       </c>
       <c r="H53" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>333333.33333333331</v>
       </c>
       <c r="I53" s="61"/>
@@ -10899,11 +12368,11 @@
         <v>21030.121932222111</v>
       </c>
       <c r="D54" s="94">
-        <f t="shared" ref="D54:E54" si="3">IFERROR($J$51*D46/SUM($C$46:$E$46)*$C$49/$J$49,0)</f>
+        <f t="shared" ref="D54:E54" si="4">IFERROR($J$51*D46/SUM($C$46:$E$46)*$C$49/$J$49,0)</f>
         <v>21030.121932222111</v>
       </c>
       <c r="E54" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20180.420035970714</v>
       </c>
       <c r="F54" s="94">
@@ -10911,11 +12380,11 @@
         <v>494190.87136929459</v>
       </c>
       <c r="G54" s="94">
-        <f t="shared" ref="G54:H54" si="4">IFERROR($J$51*G46/SUM($F$46:$H$46)*$F$49/$J$49,0)</f>
+        <f t="shared" ref="G54:H54" si="5">IFERROR($J$51*G46/SUM($F$46:$H$46)*$F$49/$J$49,0)</f>
         <v>495435.6846473029</v>
       </c>
       <c r="H54" s="94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>448132.78008298756</v>
       </c>
       <c r="I54" s="61"/>

</xml_diff>